<commit_message>
Lower cased all articles within preprocessing
</commit_message>
<xml_diff>
--- a/src/Socal/Weights/ADJ.xlsx
+++ b/src/Socal/Weights/ADJ.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sammy Caychingco\Documents\NetBeansProjects\NLPFeatures\src\weights\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sammy Caychingco\Documents\NetBeansProjects\NLPFeatures\src\Socal\Weights\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6131,11 +6131,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>